<commit_message>
completed Early Triassic occurrences?
</commit_message>
<xml_diff>
--- a/ichthyosaur-occurrences.xlsx
+++ b/ichthyosaur-occurrences.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10502"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bcm/GitHub/occurrence_data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:40009_{80ECCF8D-C5EB-8044-A516-4B53F302F998}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D80409B6-5FFF-4B41-A24B-ABF134560E78}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="14160"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="51200" windowHeight="14160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="ichthyosaur_pbdb_occs_20210420" sheetId="1" r:id="rId1"/>
@@ -4647,7 +4647,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -5186,39 +5186,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:AA653" totalsRowShown="0">
-  <autoFilter ref="A1:AA653"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:AA653" totalsRowShown="0">
+  <autoFilter ref="A1:AA653" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AA653">
     <sortCondition ref="D1:D653"/>
   </sortState>
   <tableColumns count="27">
-    <tableColumn id="1" name="occurrence_no"/>
-    <tableColumn id="5" name="collection_no"/>
-    <tableColumn id="6" name="identified_name"/>
-    <tableColumn id="10" name="accepted_name"/>
-    <tableColumn id="12" name="accepted_rank"/>
-    <tableColumn id="13" name="accepted_no"/>
-    <tableColumn id="16" name="max_ma"/>
-    <tableColumn id="17" name="min_ma"/>
-    <tableColumn id="123" name="stratigraphy"/>
-    <tableColumn id="120" name="lithostratigraphy"/>
-    <tableColumn id="121" name="biostratigraphy"/>
-    <tableColumn id="122" name="locality"/>
-    <tableColumn id="18" name="ref_author"/>
-    <tableColumn id="19" name="ref_pubyr"/>
-    <tableColumn id="30" name="lng"/>
-    <tableColumn id="31" name="lat"/>
-    <tableColumn id="119" name="specimen_no"/>
-    <tableColumn id="124" name="reference"/>
-    <tableColumn id="32" name="occurrence_comments"/>
-    <tableColumn id="43" name="paleomodel"/>
-    <tableColumn id="44" name="paleolng"/>
-    <tableColumn id="45" name="paleolat"/>
-    <tableColumn id="49" name="formation"/>
-    <tableColumn id="50" name="stratgroup"/>
-    <tableColumn id="51" name="member"/>
-    <tableColumn id="52" name="stratscale"/>
-    <tableColumn id="53" name="zone"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="occurrence_no"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="collection_no"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0000-000006000000}" name="identified_name"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0000-00000A000000}" name="accepted_name"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0000-00000C000000}" name="accepted_rank"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0000-00000D000000}" name="accepted_no"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0000-000010000000}" name="max_ma"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0000-000011000000}" name="min_ma"/>
+    <tableColumn id="123" xr3:uid="{00000000-0010-0000-0000-00007B000000}" name="stratigraphy"/>
+    <tableColumn id="120" xr3:uid="{00000000-0010-0000-0000-000078000000}" name="lithostratigraphy"/>
+    <tableColumn id="121" xr3:uid="{00000000-0010-0000-0000-000079000000}" name="biostratigraphy"/>
+    <tableColumn id="122" xr3:uid="{00000000-0010-0000-0000-00007A000000}" name="locality"/>
+    <tableColumn id="18" xr3:uid="{00000000-0010-0000-0000-000012000000}" name="ref_author"/>
+    <tableColumn id="19" xr3:uid="{00000000-0010-0000-0000-000013000000}" name="ref_pubyr"/>
+    <tableColumn id="30" xr3:uid="{00000000-0010-0000-0000-00001E000000}" name="lng"/>
+    <tableColumn id="31" xr3:uid="{00000000-0010-0000-0000-00001F000000}" name="lat"/>
+    <tableColumn id="119" xr3:uid="{00000000-0010-0000-0000-000077000000}" name="specimen_no"/>
+    <tableColumn id="124" xr3:uid="{00000000-0010-0000-0000-00007C000000}" name="reference"/>
+    <tableColumn id="32" xr3:uid="{00000000-0010-0000-0000-000020000000}" name="occurrence_comments"/>
+    <tableColumn id="43" xr3:uid="{00000000-0010-0000-0000-00002B000000}" name="paleomodel"/>
+    <tableColumn id="44" xr3:uid="{00000000-0010-0000-0000-00002C000000}" name="paleolng"/>
+    <tableColumn id="45" xr3:uid="{00000000-0010-0000-0000-00002D000000}" name="paleolat"/>
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="formation"/>
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="stratgroup"/>
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="member"/>
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="stratscale"/>
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="zone"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5520,11 +5520,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA653"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="O43" sqref="O43:P43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>